<commit_message>
#2 #28 Select image list from database
</commit_message>
<xml_diff>
--- a/desktop-app/db/data.xlsx
+++ b/desktop-app/db/data.xlsx
@@ -14,7 +14,224 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="0" uniqueCount="0"/>
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="72" count="72">
+  <x:si>
+    <x:t>id</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Application</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Started</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Closed</x:t>
+  </x:si>
+  <x:si>
+    <x:t>MousePosX</x:t>
+  </x:si>
+  <x:si>
+    <x:t>MousePosY</x:t>
+  </x:si>
+  <x:si>
+    <x:t>TotalMouseClick</x:t>
+  </x:si>
+  <x:si>
+    <x:t>MouseBtn</x:t>
+  </x:si>
+  <x:si>
+    <x:t>TotalKeyPress</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Intensity</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ScreenshotId</x:t>
+  </x:si>
+  <x:si>
+    <x:t>SequenceOfStartingMinutes</x:t>
+  </x:si>
+  <x:si>
+    <x:t>TotalActiveTime</x:t>
+  </x:si>
+  <x:si>
+    <x:t>npm start</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2017-11-11 15:29:48</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2017-11-11 15:29:52</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2017-11-11 15:31:01</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2017-11-11 15:31:05</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2017-11-11 15:34:37</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2017-11-11 15:34:45</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2017-11-11 15:34:54</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2017-11-11 15:34:56</x:t>
+  </x:si>
+  <x:si>
+    <x:t>RemoteJob</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2017-11-11 15:34:57</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2017-11-11 15:48:33</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2017-11-11 15:48:36</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2017-11-11 15:48:49</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2017-11-11 15:48:51</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2017-11-11 15:48:57</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2017-11-11 15:48:58</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2017-11-11 15:49:06</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2017-11-11 15:49:13</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2017-11-11 15:49:58</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2017-11-11 15:50:08</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2017-11-11 15:53:33</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2017-11-11 15:53:39</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2017-11-11 15:53:40</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2017-11-11 15:53:44</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Skype</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2017-11-11 16:36:14</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2017-11-11 16:36:18</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2017-11-11 16:36:20</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2017-11-11 16:47:41</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2017-11-11 16:47:43</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2017-11-11 16:47:46</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2017-11-11 16:47:47</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2017-11-11 16:47:50</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2017-11-11 16:50:40</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2017-11-11 16:50:42</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2017-11-11 16:50:43</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2017-11-11 16:51:16</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2017-11-11 16:51:19</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2017-11-11 16:51:26</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2017-11-11 16:51:27</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2017-11-11 16:51:28</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2017-11-11 16:51:29</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2017-11-11 16:51:53</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2017-11-11 16:51:55</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2017-11-11 16:52:33</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2017-11-11 16:52:34</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2017-11-11 16:53:07</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2017-11-11 16:53:09</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2017-11-11 16:58:39</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2017-11-11 16:58:42</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2017-11-11 16:58:59</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2017-11-11 16:59:05</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2017-11-11 16:59:19</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2017-11-11 16:59:26</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2017-11-11 17:00:02</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2017-11-11 17:00:08</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2017-11-11 17:01:05</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2017-11-11 17:01:10</x:t>
+  </x:si>
+</x:sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -375,7 +592,1151 @@
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:sheetData>
-    <x:row r="1" spans="1:0"/>
+    <x:row r="1" spans="1:13">
+      <x:c r="A1" s="0" t="s">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="B1" s="0" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C1" s="0" t="s">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="D1" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="E1" s="0" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="F1" s="0" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="G1" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="H1" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="I1" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="J1" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="K1" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="L1" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="M1" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2" spans="1:13">
+      <x:c r="A2" s="0" t="n">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="B2" s="0" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="C2" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="D2" s="0" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="G2" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="I2" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="J2" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="K2" s="0" t="n">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="L2" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="M2" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="3" spans="1:13">
+      <x:c r="A3" s="0" t="n">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="B3" s="0" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="C3" s="0" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="D3" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="G3" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="I3" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="J3" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="L3" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="M3" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="4" spans="1:13">
+      <x:c r="A4" s="0" t="n">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="B4" s="0" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="C4" s="0" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="D4" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="E4" s="0" t="n">
+        <x:v>521</x:v>
+      </x:c>
+      <x:c r="F4" s="0" t="n">
+        <x:v>447</x:v>
+      </x:c>
+      <x:c r="G4" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="I4" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="J4" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="K4" s="0" t="n">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="L4" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="M4" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="5" spans="1:13">
+      <x:c r="A5" s="0" t="n">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="B5" s="0" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="C5" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="D5" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="E5" s="0" t="n">
+        <x:v>544</x:v>
+      </x:c>
+      <x:c r="F5" s="0" t="n">
+        <x:v>488</x:v>
+      </x:c>
+      <x:c r="G5" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="I5" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="J5" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="K5" s="0" t="n">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="L5" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="M5" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="6" spans="1:13">
+      <x:c r="A6" s="0" t="n">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="B6" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="C6" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="D6" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E6" s="0" t="n">
+        <x:v>547</x:v>
+      </x:c>
+      <x:c r="F6" s="0" t="n">
+        <x:v>482</x:v>
+      </x:c>
+      <x:c r="G6" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="I6" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="J6" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="K6" s="0" t="n">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="L6" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="M6" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="7" spans="1:13">
+      <x:c r="A7" s="0" t="n">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="B7" s="0" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="C7" s="0" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="D7" s="0" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="G7" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="I7" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="J7" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="K7" s="0" t="n">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="L7" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="M7" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="8" spans="1:13">
+      <x:c r="A8" s="0" t="n">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="B8" s="0" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="C8" s="0" t="s">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="D8" s="0" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="E8" s="0" t="n">
+        <x:v>517</x:v>
+      </x:c>
+      <x:c r="F8" s="0" t="n">
+        <x:v>583</x:v>
+      </x:c>
+      <x:c r="G8" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="I8" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="J8" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="K8" s="0" t="n">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="L8" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="M8" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="9" spans="1:13">
+      <x:c r="A9" s="0" t="n">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="B9" s="0" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="C9" s="0" t="s">
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="D9" s="0" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="E9" s="0" t="n">
+        <x:v>576</x:v>
+      </x:c>
+      <x:c r="F9" s="0" t="n">
+        <x:v>535</x:v>
+      </x:c>
+      <x:c r="G9" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="I9" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="J9" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="K9" s="0" t="n">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="L9" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="M9" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="10" spans="1:13">
+      <x:c r="A10" s="0" t="n">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="B10" s="0" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="C10" s="0" t="s">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="D10" s="0" t="s">
+        <x:v>31</x:v>
+      </x:c>
+      <x:c r="E10" s="0" t="n">
+        <x:v>331</x:v>
+      </x:c>
+      <x:c r="F10" s="0" t="n">
+        <x:v>475</x:v>
+      </x:c>
+      <x:c r="G10" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="I10" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="J10" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="K10" s="0" t="n">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="L10" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="M10" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="11" spans="1:13">
+      <x:c r="A11" s="0" t="n">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="B11" s="0" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="C11" s="0" t="s">
+        <x:v>32</x:v>
+      </x:c>
+      <x:c r="D11" s="0" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="G11" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="I11" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="J11" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="K11" s="0" t="n">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="L11" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="M11" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="12" spans="1:13">
+      <x:c r="A12" s="0" t="n">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="B12" s="0" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="C12" s="0" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="D12" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="G12" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="I12" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="J12" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="K12" s="0" t="n">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="L12" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="M12" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="13" spans="1:13">
+      <x:c r="A13" s="0" t="n">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="B13" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="C13" s="0" t="s">
+        <x:v>36</x:v>
+      </x:c>
+      <x:c r="D13" s="0" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="G13" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="I13" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="J13" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="K13" s="0" t="n">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="L13" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="M13" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="14" spans="1:13">
+      <x:c r="A14" s="0" t="n">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="B14" s="0" t="s">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="C14" s="0" t="s">
+        <x:v>39</x:v>
+      </x:c>
+      <x:c r="D14" s="0" t="s">
+        <x:v>40</x:v>
+      </x:c>
+      <x:c r="E14" s="0" t="n">
+        <x:v>672</x:v>
+      </x:c>
+      <x:c r="F14" s="0" t="n">
+        <x:v>169</x:v>
+      </x:c>
+      <x:c r="G14" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="I14" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="J14" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="K14" s="0" t="n">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="L14" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="M14" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="15" spans="1:13">
+      <x:c r="A15" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="B15" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="C15" s="0" t="s">
+        <x:v>40</x:v>
+      </x:c>
+      <x:c r="D15" s="0" t="s">
+        <x:v>41</x:v>
+      </x:c>
+      <x:c r="E15" s="0" t="n">
+        <x:v>483</x:v>
+      </x:c>
+      <x:c r="F15" s="0" t="n">
+        <x:v>396</x:v>
+      </x:c>
+      <x:c r="G15" s="0" t="n">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="H15" s="0" t="n">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="I15" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="J15" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="K15" s="0" t="n">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="L15" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="M15" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="16" spans="1:13">
+      <x:c r="A16" s="0" t="n">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="B16" s="0" t="s">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="C16" s="0" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="D16" s="0" t="s">
+        <x:v>43</x:v>
+      </x:c>
+      <x:c r="E16" s="0" t="n">
+        <x:v>671</x:v>
+      </x:c>
+      <x:c r="F16" s="0" t="n">
+        <x:v>146</x:v>
+      </x:c>
+      <x:c r="G16" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="I16" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="J16" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="K16" s="0" t="n">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="L16" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="M16" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="17" spans="1:13">
+      <x:c r="A17" s="0" t="n">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="B17" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="C17" s="0" t="s">
+        <x:v>43</x:v>
+      </x:c>
+      <x:c r="D17" s="0" t="s">
+        <x:v>44</x:v>
+      </x:c>
+      <x:c r="E17" s="0" t="n">
+        <x:v>489</x:v>
+      </x:c>
+      <x:c r="F17" s="0" t="n">
+        <x:v>382</x:v>
+      </x:c>
+      <x:c r="G17" s="0" t="n">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="H17" s="0" t="n">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="I17" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="J17" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="K17" s="0" t="n">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="L17" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="M17" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="18" spans="1:13">
+      <x:c r="A18" s="0" t="n">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="B18" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="C18" s="0" t="s">
+        <x:v>45</x:v>
+      </x:c>
+      <x:c r="D18" s="0" t="s">
+        <x:v>46</x:v>
+      </x:c>
+      <x:c r="E18" s="0" t="n">
+        <x:v>497</x:v>
+      </x:c>
+      <x:c r="F18" s="0" t="n">
+        <x:v>439</x:v>
+      </x:c>
+      <x:c r="G18" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="I18" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="J18" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="K18" s="0" t="n">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="L18" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="M18" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="19" spans="1:13">
+      <x:c r="A19" s="0" t="n">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="B19" s="0" t="s">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="C19" s="0" t="s">
+        <x:v>47</x:v>
+      </x:c>
+      <x:c r="D19" s="0" t="s">
+        <x:v>48</x:v>
+      </x:c>
+      <x:c r="E19" s="0" t="n">
+        <x:v>523</x:v>
+      </x:c>
+      <x:c r="F19" s="0" t="n">
+        <x:v>487</x:v>
+      </x:c>
+      <x:c r="G19" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="I19" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="J19" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="K19" s="0" t="n">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="L19" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="M19" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="20" spans="1:13">
+      <x:c r="A20" s="0" t="n">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="B20" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="C20" s="0" t="s">
+        <x:v>48</x:v>
+      </x:c>
+      <x:c r="D20" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="E20" s="0" t="n">
+        <x:v>523</x:v>
+      </x:c>
+      <x:c r="F20" s="0" t="n">
+        <x:v>487</x:v>
+      </x:c>
+      <x:c r="G20" s="0" t="n">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="H20" s="0" t="n">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="I20" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="J20" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="K20" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="L20" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="M20" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="21" spans="1:13">
+      <x:c r="A21" s="0" t="n">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B21" s="0" t="s">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="C21" s="0" t="s">
+        <x:v>50</x:v>
+      </x:c>
+      <x:c r="D21" s="0" t="s">
+        <x:v>51</x:v>
+      </x:c>
+      <x:c r="E21" s="0" t="n">
+        <x:v>553</x:v>
+      </x:c>
+      <x:c r="F21" s="0" t="n">
+        <x:v>475</x:v>
+      </x:c>
+      <x:c r="G21" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="I21" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="J21" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="K21" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="L21" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="M21" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="22" spans="1:13">
+      <x:c r="A22" s="0" t="n">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="B22" s="0" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="C22" s="0" t="s">
+        <x:v>52</x:v>
+      </x:c>
+      <x:c r="D22" s="0" t="s">
+        <x:v>53</x:v>
+      </x:c>
+      <x:c r="E22" s="0" t="n">
+        <x:v>569</x:v>
+      </x:c>
+      <x:c r="F22" s="0" t="n">
+        <x:v>386</x:v>
+      </x:c>
+      <x:c r="G22" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="I22" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="J22" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="K22" s="0" t="n">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="L22" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="M22" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="23" spans="1:13">
+      <x:c r="A23" s="0" t="n">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="B23" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="C23" s="0" t="s">
+        <x:v>54</x:v>
+      </x:c>
+      <x:c r="D23" s="0" t="s">
+        <x:v>55</x:v>
+      </x:c>
+      <x:c r="G23" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="I23" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="J23" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="K23" s="0" t="n">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="L23" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="M23" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="24" spans="1:13">
+      <x:c r="A24" s="0" t="n">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="B24" s="0" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="C24" s="0" t="s">
+        <x:v>56</x:v>
+      </x:c>
+      <x:c r="D24" s="0" t="s">
+        <x:v>57</x:v>
+      </x:c>
+      <x:c r="E24" s="0" t="n">
+        <x:v>571</x:v>
+      </x:c>
+      <x:c r="F24" s="0" t="n">
+        <x:v>477</x:v>
+      </x:c>
+      <x:c r="G24" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="I24" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="J24" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="K24" s="0" t="n">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="L24" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="M24" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="25" spans="1:13">
+      <x:c r="A25" s="0" t="n">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="B25" s="0" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="C25" s="0" t="s">
+        <x:v>58</x:v>
+      </x:c>
+      <x:c r="D25" s="0" t="s">
+        <x:v>59</x:v>
+      </x:c>
+      <x:c r="E25" s="0" t="n">
+        <x:v>575</x:v>
+      </x:c>
+      <x:c r="F25" s="0" t="n">
+        <x:v>482</x:v>
+      </x:c>
+      <x:c r="G25" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="I25" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="J25" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="K25" s="0" t="n">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="L25" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="M25" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="26" spans="1:13">
+      <x:c r="A26" s="0" t="n">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="B26" s="0" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="C26" s="0" t="s">
+        <x:v>60</x:v>
+      </x:c>
+      <x:c r="D26" s="0" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="E26" s="0" t="n">
+        <x:v>594</x:v>
+      </x:c>
+      <x:c r="F26" s="0" t="n">
+        <x:v>408</x:v>
+      </x:c>
+      <x:c r="G26" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="I26" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="J26" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="K26" s="0" t="n">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="L26" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="M26" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="27" spans="1:13">
+      <x:c r="A27" s="0" t="n">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="B27" s="0" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="C27" s="0" t="s">
+        <x:v>62</x:v>
+      </x:c>
+      <x:c r="D27" s="0" t="s">
+        <x:v>63</x:v>
+      </x:c>
+      <x:c r="E27" s="0" t="n">
+        <x:v>582</x:v>
+      </x:c>
+      <x:c r="F27" s="0" t="n">
+        <x:v>494</x:v>
+      </x:c>
+      <x:c r="G27" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="I27" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="J27" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="K27" s="0" t="n">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="L27" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="M27" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="28" spans="1:13">
+      <x:c r="A28" s="0" t="n">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="B28" s="0" t="s">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="C28" s="0" t="s">
+        <x:v>64</x:v>
+      </x:c>
+      <x:c r="D28" s="0" t="s">
+        <x:v>65</x:v>
+      </x:c>
+      <x:c r="E28" s="0" t="n">
+        <x:v>567</x:v>
+      </x:c>
+      <x:c r="F28" s="0" t="n">
+        <x:v>403</x:v>
+      </x:c>
+      <x:c r="G28" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="I28" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="J28" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="K28" s="0" t="n">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="L28" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="M28" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="29" spans="1:13">
+      <x:c r="A29" s="0" t="n">
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="B29" s="0" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="C29" s="0" t="s">
+        <x:v>66</x:v>
+      </x:c>
+      <x:c r="D29" s="0" t="s">
+        <x:v>67</x:v>
+      </x:c>
+      <x:c r="E29" s="0" t="n">
+        <x:v>578</x:v>
+      </x:c>
+      <x:c r="F29" s="0" t="n">
+        <x:v>452</x:v>
+      </x:c>
+      <x:c r="G29" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="I29" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="J29" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="K29" s="0" t="n">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="L29" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="M29" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="30" spans="1:13">
+      <x:c r="A30" s="0" t="n">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="B30" s="0" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="C30" s="0" t="s">
+        <x:v>68</x:v>
+      </x:c>
+      <x:c r="D30" s="0" t="s">
+        <x:v>69</x:v>
+      </x:c>
+      <x:c r="E30" s="0" t="n">
+        <x:v>518</x:v>
+      </x:c>
+      <x:c r="F30" s="0" t="n">
+        <x:v>450</x:v>
+      </x:c>
+      <x:c r="G30" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="I30" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="J30" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="K30" s="0" t="n">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="L30" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="M30" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="31" spans="1:13">
+      <x:c r="A31" s="0" t="n">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="B31" s="0" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="C31" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="D31" s="0" t="s">
+        <x:v>71</x:v>
+      </x:c>
+      <x:c r="E31" s="0" t="n">
+        <x:v>571</x:v>
+      </x:c>
+      <x:c r="F31" s="0" t="n">
+        <x:v>453</x:v>
+      </x:c>
+      <x:c r="G31" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="I31" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="J31" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="K31" s="0" t="n">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="L31" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="M31" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
   </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>

</xml_diff>

<commit_message>
#2 #29 Generate images from selected list
</commit_message>
<xml_diff>
--- a/desktop-app/db/data.xlsx
+++ b/desktop-app/db/data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="72" count="72">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="50" count="50">
   <x:si>
     <x:t>id</x:t>
   </x:si>
@@ -55,181 +55,115 @@
     <x:t>TotalActiveTime</x:t>
   </x:si>
   <x:si>
+    <x:t>RemoteJob</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2017-11-11 19:00:37</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2017-11-11 19:00:41</x:t>
+  </x:si>
+  <x:si>
     <x:t>npm start</x:t>
   </x:si>
   <x:si>
-    <x:t>2017-11-11 15:29:48</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2017-11-11 15:29:52</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2017-11-11 15:31:01</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2017-11-11 15:31:05</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2017-11-11 15:34:37</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2017-11-11 15:34:45</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2017-11-11 15:34:54</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2017-11-11 15:34:56</x:t>
-  </x:si>
-  <x:si>
-    <x:t>RemoteJob</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2017-11-11 15:34:57</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2017-11-11 15:48:33</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2017-11-11 15:48:36</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2017-11-11 15:48:49</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2017-11-11 15:48:51</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2017-11-11 15:48:57</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2017-11-11 15:48:58</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2017-11-11 15:49:06</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2017-11-11 15:49:13</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2017-11-11 15:49:58</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2017-11-11 15:50:08</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2017-11-11 15:53:33</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2017-11-11 15:53:39</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2017-11-11 15:53:40</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2017-11-11 15:53:44</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Skype</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2017-11-11 16:36:14</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2017-11-11 16:36:18</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2017-11-11 16:36:20</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2017-11-11 16:47:41</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2017-11-11 16:47:43</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2017-11-11 16:47:46</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2017-11-11 16:47:47</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2017-11-11 16:47:50</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2017-11-11 16:50:40</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2017-11-11 16:50:42</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2017-11-11 16:50:43</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2017-11-11 16:51:16</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2017-11-11 16:51:19</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2017-11-11 16:51:26</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2017-11-11 16:51:27</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2017-11-11 16:51:28</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2017-11-11 16:51:29</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2017-11-11 16:51:53</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2017-11-11 16:51:55</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2017-11-11 16:52:33</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2017-11-11 16:52:34</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2017-11-11 16:53:07</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2017-11-11 16:53:09</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2017-11-11 16:58:39</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2017-11-11 16:58:42</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2017-11-11 16:58:59</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2017-11-11 16:59:05</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2017-11-11 16:59:19</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2017-11-11 16:59:26</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2017-11-11 17:00:02</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2017-11-11 17:00:08</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2017-11-11 17:01:05</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2017-11-11 17:01:10</x:t>
+    <x:t>2017-11-11 19:00:47</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2017-11-11 19:00:48</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2017-11-11 19:00:51</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2017-11-11 19:02:30</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2017-11-11 19:02:36</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2017-11-11 19:03:00</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2017-11-11 19:03:08</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2017-11-11 19:03:34</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2017-11-11 19:03:38</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2017-11-11 19:09:43</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2017-11-11 19:09:48</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2017-11-11 19:09:51</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2017-11-11 19:13:25</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2017-11-11 19:13:36</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2017-11-11 19:17:22</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2017-11-11 19:17:28</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2017-11-11 19:18:19</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2017-11-11 19:18:28</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2017-11-11 19:20:42</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2017-11-11 19:20:48</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2017-11-11 19:21:08</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2017-11-11 19:25:17</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2017-11-11 19:25:21</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2017-11-11 19:25:40</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2017-11-11 19:25:45</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2017-11-11 19:26:40</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2017-11-11 19:26:41</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2017-11-11 19:26:59</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2017-11-11 19:27:13</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2017-11-11 19:27:30</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2017-11-11 19:27:40</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2017-11-11 19:28:48</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2017-11-11 19:28:57</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -646,11 +580,20 @@
       <x:c r="D2" s="0" t="s">
         <x:v>15</x:v>
       </x:c>
+      <x:c r="E2" s="0" t="n">
+        <x:v>441</x:v>
+      </x:c>
+      <x:c r="F2" s="0" t="n">
+        <x:v>459</x:v>
+      </x:c>
       <x:c r="G2" s="0" t="n">
-        <x:v>0</x:v>
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="H2" s="0" t="n">
+        <x:v>1</x:v>
       </x:c>
       <x:c r="I2" s="0" t="n">
-        <x:v>0</x:v>
+        <x:v>1</x:v>
       </x:c>
       <x:c r="J2" s="0" t="n">
         <x:v>0</x:v>
@@ -670,13 +613,19 @@
         <x:v>2</x:v>
       </x:c>
       <x:c r="B3" s="0" t="s">
-        <x:v>13</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="C3" s="0" t="s">
-        <x:v>16</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="D3" s="0" t="s">
-        <x:v>17</x:v>
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="E3" s="0" t="n">
+        <x:v>483</x:v>
+      </x:c>
+      <x:c r="F3" s="0" t="n">
+        <x:v>423</x:v>
       </x:c>
       <x:c r="G3" s="0" t="n">
         <x:v>0</x:v>
@@ -686,6 +635,9 @@
       </x:c>
       <x:c r="J3" s="0" t="n">
         <x:v>0</x:v>
+      </x:c>
+      <x:c r="K3" s="0" t="n">
+        <x:v>1</x:v>
       </x:c>
       <x:c r="L3" s="0" t="n">
         <x:v>0</x:v>
@@ -708,13 +660,16 @@
         <x:v>19</x:v>
       </x:c>
       <x:c r="E4" s="0" t="n">
-        <x:v>521</x:v>
+        <x:v>469</x:v>
       </x:c>
       <x:c r="F4" s="0" t="n">
-        <x:v>447</x:v>
+        <x:v>389</x:v>
       </x:c>
       <x:c r="G4" s="0" t="n">
-        <x:v>0</x:v>
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="H4" s="0" t="n">
+        <x:v>1</x:v>
       </x:c>
       <x:c r="I4" s="0" t="n">
         <x:v>0</x:v>
@@ -723,7 +678,7 @@
         <x:v>0</x:v>
       </x:c>
       <x:c r="K4" s="0" t="n">
-        <x:v>1</x:v>
+        <x:v>2</x:v>
       </x:c>
       <x:c r="L4" s="0" t="n">
         <x:v>0</x:v>
@@ -737,7 +692,7 @@
         <x:v>4</x:v>
       </x:c>
       <x:c r="B5" s="0" t="s">
-        <x:v>13</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="C5" s="0" t="s">
         <x:v>20</x:v>
@@ -746,10 +701,10 @@
         <x:v>21</x:v>
       </x:c>
       <x:c r="E5" s="0" t="n">
-        <x:v>544</x:v>
+        <x:v>551</x:v>
       </x:c>
       <x:c r="F5" s="0" t="n">
-        <x:v>488</x:v>
+        <x:v>453</x:v>
       </x:c>
       <x:c r="G5" s="0" t="n">
         <x:v>0</x:v>
@@ -775,19 +730,19 @@
         <x:v>5</x:v>
       </x:c>
       <x:c r="B6" s="0" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="C6" s="0" t="s">
         <x:v>22</x:v>
-      </x:c>
-      <x:c r="C6" s="0" t="s">
-        <x:v>21</x:v>
       </x:c>
       <x:c r="D6" s="0" t="s">
         <x:v>23</x:v>
       </x:c>
       <x:c r="E6" s="0" t="n">
-        <x:v>547</x:v>
+        <x:v>551</x:v>
       </x:c>
       <x:c r="F6" s="0" t="n">
-        <x:v>482</x:v>
+        <x:v>440</x:v>
       </x:c>
       <x:c r="G6" s="0" t="n">
         <x:v>0</x:v>
@@ -813,7 +768,7 @@
         <x:v>6</x:v>
       </x:c>
       <x:c r="B7" s="0" t="s">
-        <x:v>13</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="C7" s="0" t="s">
         <x:v>24</x:v>
@@ -821,6 +776,12 @@
       <x:c r="D7" s="0" t="s">
         <x:v>25</x:v>
       </x:c>
+      <x:c r="E7" s="0" t="n">
+        <x:v>512</x:v>
+      </x:c>
+      <x:c r="F7" s="0" t="n">
+        <x:v>358</x:v>
+      </x:c>
       <x:c r="G7" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
@@ -831,7 +792,7 @@
         <x:v>0</x:v>
       </x:c>
       <x:c r="K7" s="0" t="n">
-        <x:v>3</x:v>
+        <x:v>4</x:v>
       </x:c>
       <x:c r="L7" s="0" t="n">
         <x:v>0</x:v>
@@ -845,7 +806,7 @@
         <x:v>7</x:v>
       </x:c>
       <x:c r="B8" s="0" t="s">
-        <x:v>13</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="C8" s="0" t="s">
         <x:v>26</x:v>
@@ -854,10 +815,10 @@
         <x:v>27</x:v>
       </x:c>
       <x:c r="E8" s="0" t="n">
-        <x:v>517</x:v>
+        <x:v>1129</x:v>
       </x:c>
       <x:c r="F8" s="0" t="n">
-        <x:v>583</x:v>
+        <x:v>595</x:v>
       </x:c>
       <x:c r="G8" s="0" t="n">
         <x:v>0</x:v>
@@ -869,7 +830,7 @@
         <x:v>0</x:v>
       </x:c>
       <x:c r="K8" s="0" t="n">
-        <x:v>4</x:v>
+        <x:v>5</x:v>
       </x:c>
       <x:c r="L8" s="0" t="n">
         <x:v>0</x:v>
@@ -886,19 +847,22 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="C9" s="0" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="D9" s="0" t="s">
         <x:v>28</x:v>
       </x:c>
-      <x:c r="D9" s="0" t="s">
-        <x:v>29</x:v>
-      </x:c>
       <x:c r="E9" s="0" t="n">
-        <x:v>576</x:v>
+        <x:v>545</x:v>
       </x:c>
       <x:c r="F9" s="0" t="n">
-        <x:v>535</x:v>
+        <x:v>359</x:v>
       </x:c>
       <x:c r="G9" s="0" t="n">
-        <x:v>0</x:v>
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="H9" s="0" t="n">
+        <x:v>1</x:v>
       </x:c>
       <x:c r="I9" s="0" t="n">
         <x:v>0</x:v>
@@ -907,7 +871,7 @@
         <x:v>0</x:v>
       </x:c>
       <x:c r="K9" s="0" t="n">
-        <x:v>5</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="L9" s="0" t="n">
         <x:v>0</x:v>
@@ -921,19 +885,19 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="B10" s="0" t="s">
-        <x:v>13</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="C10" s="0" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="D10" s="0" t="s">
         <x:v>30</x:v>
       </x:c>
-      <x:c r="D10" s="0" t="s">
-        <x:v>31</x:v>
-      </x:c>
       <x:c r="E10" s="0" t="n">
-        <x:v>331</x:v>
+        <x:v>508</x:v>
       </x:c>
       <x:c r="F10" s="0" t="n">
-        <x:v>475</x:v>
+        <x:v>337</x:v>
       </x:c>
       <x:c r="G10" s="0" t="n">
         <x:v>0</x:v>
@@ -959,13 +923,19 @@
         <x:v>10</x:v>
       </x:c>
       <x:c r="B11" s="0" t="s">
-        <x:v>13</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="C11" s="0" t="s">
+        <x:v>31</x:v>
+      </x:c>
+      <x:c r="D11" s="0" t="s">
         <x:v>32</x:v>
       </x:c>
-      <x:c r="D11" s="0" t="s">
-        <x:v>33</x:v>
+      <x:c r="E11" s="0" t="n">
+        <x:v>546</x:v>
+      </x:c>
+      <x:c r="F11" s="0" t="n">
+        <x:v>487</x:v>
       </x:c>
       <x:c r="G11" s="0" t="n">
         <x:v>0</x:v>
@@ -991,13 +961,19 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="B12" s="0" t="s">
-        <x:v>13</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="C12" s="0" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="D12" s="0" t="s">
         <x:v>34</x:v>
       </x:c>
-      <x:c r="D12" s="0" t="s">
-        <x:v>35</x:v>
+      <x:c r="E12" s="0" t="n">
+        <x:v>632</x:v>
+      </x:c>
+      <x:c r="F12" s="0" t="n">
+        <x:v>522</x:v>
       </x:c>
       <x:c r="G12" s="0" t="n">
         <x:v>0</x:v>
@@ -1023,13 +999,19 @@
         <x:v>12</x:v>
       </x:c>
       <x:c r="B13" s="0" t="s">
-        <x:v>22</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="C13" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="D13" s="0" t="s">
         <x:v>36</x:v>
       </x:c>
-      <x:c r="D13" s="0" t="s">
-        <x:v>37</x:v>
+      <x:c r="E13" s="0" t="n">
+        <x:v>951</x:v>
+      </x:c>
+      <x:c r="F13" s="0" t="n">
+        <x:v>468</x:v>
       </x:c>
       <x:c r="G13" s="0" t="n">
         <x:v>0</x:v>
@@ -1055,22 +1037,25 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="B14" s="0" t="s">
-        <x:v>38</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="C14" s="0" t="s">
-        <x:v>39</x:v>
+        <x:v>36</x:v>
       </x:c>
       <x:c r="D14" s="0" t="s">
-        <x:v>40</x:v>
+        <x:v>37</x:v>
       </x:c>
       <x:c r="E14" s="0" t="n">
-        <x:v>672</x:v>
+        <x:v>484</x:v>
       </x:c>
       <x:c r="F14" s="0" t="n">
-        <x:v>169</x:v>
+        <x:v>461</x:v>
       </x:c>
       <x:c r="G14" s="0" t="n">
-        <x:v>0</x:v>
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="H14" s="0" t="n">
+        <x:v>1</x:v>
       </x:c>
       <x:c r="I14" s="0" t="n">
         <x:v>0</x:v>
@@ -1093,25 +1078,22 @@
         <x:v>14</x:v>
       </x:c>
       <x:c r="B15" s="0" t="s">
-        <x:v>22</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="C15" s="0" t="s">
-        <x:v>40</x:v>
+        <x:v>38</x:v>
       </x:c>
       <x:c r="D15" s="0" t="s">
-        <x:v>41</x:v>
+        <x:v>39</x:v>
       </x:c>
       <x:c r="E15" s="0" t="n">
-        <x:v>483</x:v>
+        <x:v>597</x:v>
       </x:c>
       <x:c r="F15" s="0" t="n">
-        <x:v>396</x:v>
+        <x:v>519</x:v>
       </x:c>
       <x:c r="G15" s="0" t="n">
-        <x:v>4</x:v>
-      </x:c>
-      <x:c r="H15" s="0" t="n">
-        <x:v>1</x:v>
+        <x:v>0</x:v>
       </x:c>
       <x:c r="I15" s="0" t="n">
         <x:v>0</x:v>
@@ -1120,7 +1102,7 @@
         <x:v>0</x:v>
       </x:c>
       <x:c r="K15" s="0" t="n">
-        <x:v>11</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="L15" s="0" t="n">
         <x:v>0</x:v>
@@ -1134,19 +1116,19 @@
         <x:v>15</x:v>
       </x:c>
       <x:c r="B16" s="0" t="s">
-        <x:v>38</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="C16" s="0" t="s">
-        <x:v>42</x:v>
+        <x:v>40</x:v>
       </x:c>
       <x:c r="D16" s="0" t="s">
-        <x:v>43</x:v>
+        <x:v>41</x:v>
       </x:c>
       <x:c r="E16" s="0" t="n">
-        <x:v>671</x:v>
+        <x:v>568</x:v>
       </x:c>
       <x:c r="F16" s="0" t="n">
-        <x:v>146</x:v>
+        <x:v>534</x:v>
       </x:c>
       <x:c r="G16" s="0" t="n">
         <x:v>0</x:v>
@@ -1172,25 +1154,22 @@
         <x:v>16</x:v>
       </x:c>
       <x:c r="B17" s="0" t="s">
-        <x:v>22</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="C17" s="0" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="D17" s="0" t="s">
         <x:v>43</x:v>
       </x:c>
-      <x:c r="D17" s="0" t="s">
-        <x:v>44</x:v>
-      </x:c>
       <x:c r="E17" s="0" t="n">
-        <x:v>489</x:v>
+        <x:v>515</x:v>
       </x:c>
       <x:c r="F17" s="0" t="n">
-        <x:v>382</x:v>
+        <x:v>414</x:v>
       </x:c>
       <x:c r="G17" s="0" t="n">
-        <x:v>2</x:v>
-      </x:c>
-      <x:c r="H17" s="0" t="n">
-        <x:v>1</x:v>
+        <x:v>0</x:v>
       </x:c>
       <x:c r="I17" s="0" t="n">
         <x:v>0</x:v>
@@ -1213,31 +1192,31 @@
         <x:v>17</x:v>
       </x:c>
       <x:c r="B18" s="0" t="s">
-        <x:v>22</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="C18" s="0" t="s">
+        <x:v>44</x:v>
+      </x:c>
+      <x:c r="D18" s="0" t="s">
         <x:v>45</x:v>
       </x:c>
-      <x:c r="D18" s="0" t="s">
-        <x:v>46</x:v>
-      </x:c>
       <x:c r="E18" s="0" t="n">
-        <x:v>497</x:v>
+        <x:v>642</x:v>
       </x:c>
       <x:c r="F18" s="0" t="n">
-        <x:v>439</x:v>
+        <x:v>484</x:v>
       </x:c>
       <x:c r="G18" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="I18" s="0" t="n">
-        <x:v>0</x:v>
+        <x:v>4</x:v>
       </x:c>
       <x:c r="J18" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="K18" s="0" t="n">
-        <x:v>12</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="L18" s="0" t="n">
         <x:v>0</x:v>
@@ -1251,31 +1230,31 @@
         <x:v>18</x:v>
       </x:c>
       <x:c r="B19" s="0" t="s">
-        <x:v>38</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="C19" s="0" t="s">
+        <x:v>46</x:v>
+      </x:c>
+      <x:c r="D19" s="0" t="s">
         <x:v>47</x:v>
       </x:c>
-      <x:c r="D19" s="0" t="s">
-        <x:v>48</x:v>
-      </x:c>
       <x:c r="E19" s="0" t="n">
-        <x:v>523</x:v>
+        <x:v>620</x:v>
       </x:c>
       <x:c r="F19" s="0" t="n">
-        <x:v>487</x:v>
+        <x:v>533</x:v>
       </x:c>
       <x:c r="G19" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="I19" s="0" t="n">
-        <x:v>0</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="J19" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="K19" s="0" t="n">
-        <x:v>13</x:v>
+        <x:v>14</x:v>
       </x:c>
       <x:c r="L19" s="0" t="n">
         <x:v>0</x:v>
@@ -1289,7 +1268,7 @@
         <x:v>19</x:v>
       </x:c>
       <x:c r="B20" s="0" t="s">
-        <x:v>22</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="C20" s="0" t="s">
         <x:v>48</x:v>
@@ -1298,442 +1277,27 @@
         <x:v>49</x:v>
       </x:c>
       <x:c r="E20" s="0" t="n">
-        <x:v>523</x:v>
+        <x:v>542</x:v>
       </x:c>
       <x:c r="F20" s="0" t="n">
-        <x:v>487</x:v>
+        <x:v>507</x:v>
       </x:c>
       <x:c r="G20" s="0" t="n">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="H20" s="0" t="n">
-        <x:v>1</x:v>
+        <x:v>0</x:v>
       </x:c>
       <x:c r="I20" s="0" t="n">
-        <x:v>0</x:v>
+        <x:v>4</x:v>
       </x:c>
       <x:c r="J20" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="K20" s="0" t="n">
-        <x:v>14</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="L20" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="M20" s="0" t="n">
-        <x:v>0</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="21" spans="1:13">
-      <x:c r="A21" s="0" t="n">
-        <x:v>20</x:v>
-      </x:c>
-      <x:c r="B21" s="0" t="s">
-        <x:v>38</x:v>
-      </x:c>
-      <x:c r="C21" s="0" t="s">
-        <x:v>50</x:v>
-      </x:c>
-      <x:c r="D21" s="0" t="s">
-        <x:v>51</x:v>
-      </x:c>
-      <x:c r="E21" s="0" t="n">
-        <x:v>553</x:v>
-      </x:c>
-      <x:c r="F21" s="0" t="n">
-        <x:v>475</x:v>
-      </x:c>
-      <x:c r="G21" s="0" t="n">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="I21" s="0" t="n">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="J21" s="0" t="n">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="K21" s="0" t="n">
-        <x:v>14</x:v>
-      </x:c>
-      <x:c r="L21" s="0" t="n">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="M21" s="0" t="n">
-        <x:v>0</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="22" spans="1:13">
-      <x:c r="A22" s="0" t="n">
-        <x:v>21</x:v>
-      </x:c>
-      <x:c r="B22" s="0" t="s">
-        <x:v>13</x:v>
-      </x:c>
-      <x:c r="C22" s="0" t="s">
-        <x:v>52</x:v>
-      </x:c>
-      <x:c r="D22" s="0" t="s">
-        <x:v>53</x:v>
-      </x:c>
-      <x:c r="E22" s="0" t="n">
-        <x:v>569</x:v>
-      </x:c>
-      <x:c r="F22" s="0" t="n">
-        <x:v>386</x:v>
-      </x:c>
-      <x:c r="G22" s="0" t="n">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="I22" s="0" t="n">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="J22" s="0" t="n">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="K22" s="0" t="n">
-        <x:v>15</x:v>
-      </x:c>
-      <x:c r="L22" s="0" t="n">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="M22" s="0" t="n">
-        <x:v>0</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="23" spans="1:13">
-      <x:c r="A23" s="0" t="n">
-        <x:v>22</x:v>
-      </x:c>
-      <x:c r="B23" s="0" t="s">
-        <x:v>22</x:v>
-      </x:c>
-      <x:c r="C23" s="0" t="s">
-        <x:v>54</x:v>
-      </x:c>
-      <x:c r="D23" s="0" t="s">
-        <x:v>55</x:v>
-      </x:c>
-      <x:c r="G23" s="0" t="n">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="I23" s="0" t="n">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="J23" s="0" t="n">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="K23" s="0" t="n">
-        <x:v>16</x:v>
-      </x:c>
-      <x:c r="L23" s="0" t="n">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="M23" s="0" t="n">
-        <x:v>0</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="24" spans="1:13">
-      <x:c r="A24" s="0" t="n">
-        <x:v>23</x:v>
-      </x:c>
-      <x:c r="B24" s="0" t="s">
-        <x:v>13</x:v>
-      </x:c>
-      <x:c r="C24" s="0" t="s">
-        <x:v>56</x:v>
-      </x:c>
-      <x:c r="D24" s="0" t="s">
-        <x:v>57</x:v>
-      </x:c>
-      <x:c r="E24" s="0" t="n">
-        <x:v>571</x:v>
-      </x:c>
-      <x:c r="F24" s="0" t="n">
-        <x:v>477</x:v>
-      </x:c>
-      <x:c r="G24" s="0" t="n">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="I24" s="0" t="n">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="J24" s="0" t="n">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="K24" s="0" t="n">
-        <x:v>17</x:v>
-      </x:c>
-      <x:c r="L24" s="0" t="n">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="M24" s="0" t="n">
-        <x:v>0</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="25" spans="1:13">
-      <x:c r="A25" s="0" t="n">
-        <x:v>24</x:v>
-      </x:c>
-      <x:c r="B25" s="0" t="s">
-        <x:v>13</x:v>
-      </x:c>
-      <x:c r="C25" s="0" t="s">
-        <x:v>58</x:v>
-      </x:c>
-      <x:c r="D25" s="0" t="s">
-        <x:v>59</x:v>
-      </x:c>
-      <x:c r="E25" s="0" t="n">
-        <x:v>575</x:v>
-      </x:c>
-      <x:c r="F25" s="0" t="n">
-        <x:v>482</x:v>
-      </x:c>
-      <x:c r="G25" s="0" t="n">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="I25" s="0" t="n">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="J25" s="0" t="n">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="K25" s="0" t="n">
-        <x:v>18</x:v>
-      </x:c>
-      <x:c r="L25" s="0" t="n">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="M25" s="0" t="n">
-        <x:v>0</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="26" spans="1:13">
-      <x:c r="A26" s="0" t="n">
-        <x:v>25</x:v>
-      </x:c>
-      <x:c r="B26" s="0" t="s">
-        <x:v>13</x:v>
-      </x:c>
-      <x:c r="C26" s="0" t="s">
-        <x:v>60</x:v>
-      </x:c>
-      <x:c r="D26" s="0" t="s">
-        <x:v>61</x:v>
-      </x:c>
-      <x:c r="E26" s="0" t="n">
-        <x:v>594</x:v>
-      </x:c>
-      <x:c r="F26" s="0" t="n">
-        <x:v>408</x:v>
-      </x:c>
-      <x:c r="G26" s="0" t="n">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="I26" s="0" t="n">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="J26" s="0" t="n">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="K26" s="0" t="n">
-        <x:v>19</x:v>
-      </x:c>
-      <x:c r="L26" s="0" t="n">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="M26" s="0" t="n">
-        <x:v>0</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="27" spans="1:13">
-      <x:c r="A27" s="0" t="n">
-        <x:v>26</x:v>
-      </x:c>
-      <x:c r="B27" s="0" t="s">
-        <x:v>13</x:v>
-      </x:c>
-      <x:c r="C27" s="0" t="s">
-        <x:v>62</x:v>
-      </x:c>
-      <x:c r="D27" s="0" t="s">
-        <x:v>63</x:v>
-      </x:c>
-      <x:c r="E27" s="0" t="n">
-        <x:v>582</x:v>
-      </x:c>
-      <x:c r="F27" s="0" t="n">
-        <x:v>494</x:v>
-      </x:c>
-      <x:c r="G27" s="0" t="n">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="I27" s="0" t="n">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="J27" s="0" t="n">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="K27" s="0" t="n">
-        <x:v>20</x:v>
-      </x:c>
-      <x:c r="L27" s="0" t="n">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="M27" s="0" t="n">
-        <x:v>0</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="28" spans="1:13">
-      <x:c r="A28" s="0" t="n">
-        <x:v>27</x:v>
-      </x:c>
-      <x:c r="B28" s="0" t="s">
-        <x:v>38</x:v>
-      </x:c>
-      <x:c r="C28" s="0" t="s">
-        <x:v>64</x:v>
-      </x:c>
-      <x:c r="D28" s="0" t="s">
-        <x:v>65</x:v>
-      </x:c>
-      <x:c r="E28" s="0" t="n">
-        <x:v>567</x:v>
-      </x:c>
-      <x:c r="F28" s="0" t="n">
-        <x:v>403</x:v>
-      </x:c>
-      <x:c r="G28" s="0" t="n">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="I28" s="0" t="n">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="J28" s="0" t="n">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="K28" s="0" t="n">
-        <x:v>21</x:v>
-      </x:c>
-      <x:c r="L28" s="0" t="n">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="M28" s="0" t="n">
-        <x:v>0</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="29" spans="1:13">
-      <x:c r="A29" s="0" t="n">
-        <x:v>28</x:v>
-      </x:c>
-      <x:c r="B29" s="0" t="s">
-        <x:v>13</x:v>
-      </x:c>
-      <x:c r="C29" s="0" t="s">
-        <x:v>66</x:v>
-      </x:c>
-      <x:c r="D29" s="0" t="s">
-        <x:v>67</x:v>
-      </x:c>
-      <x:c r="E29" s="0" t="n">
-        <x:v>578</x:v>
-      </x:c>
-      <x:c r="F29" s="0" t="n">
-        <x:v>452</x:v>
-      </x:c>
-      <x:c r="G29" s="0" t="n">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="I29" s="0" t="n">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="J29" s="0" t="n">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="K29" s="0" t="n">
-        <x:v>22</x:v>
-      </x:c>
-      <x:c r="L29" s="0" t="n">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="M29" s="0" t="n">
-        <x:v>0</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="30" spans="1:13">
-      <x:c r="A30" s="0" t="n">
-        <x:v>29</x:v>
-      </x:c>
-      <x:c r="B30" s="0" t="s">
-        <x:v>13</x:v>
-      </x:c>
-      <x:c r="C30" s="0" t="s">
-        <x:v>68</x:v>
-      </x:c>
-      <x:c r="D30" s="0" t="s">
-        <x:v>69</x:v>
-      </x:c>
-      <x:c r="E30" s="0" t="n">
-        <x:v>518</x:v>
-      </x:c>
-      <x:c r="F30" s="0" t="n">
-        <x:v>450</x:v>
-      </x:c>
-      <x:c r="G30" s="0" t="n">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="I30" s="0" t="n">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="J30" s="0" t="n">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="K30" s="0" t="n">
-        <x:v>23</x:v>
-      </x:c>
-      <x:c r="L30" s="0" t="n">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="M30" s="0" t="n">
-        <x:v>0</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="31" spans="1:13">
-      <x:c r="A31" s="0" t="n">
-        <x:v>30</x:v>
-      </x:c>
-      <x:c r="B31" s="0" t="s">
-        <x:v>13</x:v>
-      </x:c>
-      <x:c r="C31" s="0" t="s">
-        <x:v>70</x:v>
-      </x:c>
-      <x:c r="D31" s="0" t="s">
-        <x:v>71</x:v>
-      </x:c>
-      <x:c r="E31" s="0" t="n">
-        <x:v>571</x:v>
-      </x:c>
-      <x:c r="F31" s="0" t="n">
-        <x:v>453</x:v>
-      </x:c>
-      <x:c r="G31" s="0" t="n">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="I31" s="0" t="n">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="J31" s="0" t="n">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="K31" s="0" t="n">
-        <x:v>24</x:v>
-      </x:c>
-      <x:c r="L31" s="0" t="n">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="M31" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
     </x:row>

</xml_diff>

<commit_message>
Add a pop up window for sending start or end email
</commit_message>
<xml_diff>
--- a/desktop-app/db/data.xlsx
+++ b/desktop-app/db/data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="96" count="96">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="143" count="143">
   <x:si>
     <x:t>id</x:t>
   </x:si>
@@ -302,6 +302,147 @@
   </x:si>
   <x:si>
     <x:t>2017-11-12 09:03:38</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2017-11-12 09:03:44</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2017-11-12 09:03:48</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2017-11-12 09:27:23</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2017-11-12 09:27:30</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2017-11-12 09:27:33</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2017-11-12 09:27:52</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2017-11-12 09:27:53</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2017-11-12 09:28:00</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2017-11-12 09:28:37</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2017-11-12 09:28:39</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2017-11-12 09:28:51</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2017-11-12 09:29:12</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2017-11-12 09:29:14</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2017-11-12 09:29:18</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2017-11-12 09:29:37</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2017-11-12 09:29:38</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2017-11-12 09:30:07</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2017-11-12 09:30:44</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2017-11-12 09:30:46</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2017-11-12 09:31:11</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2017-11-12 09:31:13</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2017-11-12 09:37:17</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2017-11-12 09:37:18</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2017-11-12 09:37:40</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2017-11-12 09:37:42</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2017-11-12 09:38:50</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2017-11-12 09:38:52</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2017-11-12 09:39:55</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2017-11-12 09:39:59</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2017-11-12 09:40:13</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2017-11-12 09:40:16</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2017-11-12 09:40:31</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2017-11-12 09:40:34</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2017-11-12 09:40:44</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2017-11-12 09:40:53</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2017-11-12 09:41:21</x:t>
+  </x:si>
+  <x:si>
+    <x:t>book-manager</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2017-11-12 09:41:26</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2017-11-12 09:41:29</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2017-11-12 09:41:30</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2017-11-12 09:41:32</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2017-11-12 09:41:52</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2017-11-12 09:41:57</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2017-11-12 09:46:47</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2017-11-12 09:46:50</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2017-11-12 10:06:41</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2017-11-12 10:06:43</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -2404,6 +2545,1135 @@
         <x:v>0</x:v>
       </x:c>
     </x:row>
+    <x:row r="46" spans="1:13">
+      <x:c r="A46" s="0" t="n">
+        <x:v>45</x:v>
+      </x:c>
+      <x:c r="B46" s="0" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="C46" s="0" t="s">
+        <x:v>95</x:v>
+      </x:c>
+      <x:c r="D46" s="0" t="s">
+        <x:v>95</x:v>
+      </x:c>
+      <x:c r="E46" s="0" t="n">
+        <x:v>569</x:v>
+      </x:c>
+      <x:c r="F46" s="0" t="n">
+        <x:v>473</x:v>
+      </x:c>
+      <x:c r="G46" s="0" t="n">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="H46" s="0" t="n">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="I46" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="J46" s="0" t="n">
+        <x:v>0.33</x:v>
+      </x:c>
+      <x:c r="K46" s="0" t="n">
+        <x:v>36</x:v>
+      </x:c>
+      <x:c r="L46" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="M46" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="47" spans="1:13">
+      <x:c r="A47" s="0" t="n">
+        <x:v>46</x:v>
+      </x:c>
+      <x:c r="B47" s="0" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="C47" s="0" t="s">
+        <x:v>96</x:v>
+      </x:c>
+      <x:c r="D47" s="0" t="s">
+        <x:v>97</x:v>
+      </x:c>
+      <x:c r="E47" s="0" t="n">
+        <x:v>420</x:v>
+      </x:c>
+      <x:c r="F47" s="0" t="n">
+        <x:v>416</x:v>
+      </x:c>
+      <x:c r="G47" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="I47" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="J47" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="K47" s="0" t="n">
+        <x:v>36</x:v>
+      </x:c>
+      <x:c r="L47" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="M47" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="48" spans="1:13">
+      <x:c r="A48" s="0" t="n">
+        <x:v>47</x:v>
+      </x:c>
+      <x:c r="B48" s="0" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="C48" s="0" t="s">
+        <x:v>98</x:v>
+      </x:c>
+      <x:c r="D48" s="0" t="s">
+        <x:v>99</x:v>
+      </x:c>
+      <x:c r="E48" s="0" t="n">
+        <x:v>537</x:v>
+      </x:c>
+      <x:c r="F48" s="0" t="n">
+        <x:v>494</x:v>
+      </x:c>
+      <x:c r="G48" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="I48" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="J48" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="K48" s="0" t="n">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="L48" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="M48" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="49" spans="1:13">
+      <x:c r="A49" s="0" t="n">
+        <x:v>48</x:v>
+      </x:c>
+      <x:c r="B49" s="0" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="C49" s="0" t="s">
+        <x:v>99</x:v>
+      </x:c>
+      <x:c r="D49" s="0" t="s">
+        <x:v>100</x:v>
+      </x:c>
+      <x:c r="E49" s="0" t="n">
+        <x:v>549</x:v>
+      </x:c>
+      <x:c r="F49" s="0" t="n">
+        <x:v>472</x:v>
+      </x:c>
+      <x:c r="G49" s="0" t="n">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="H49" s="0" t="n">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="I49" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="J49" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="K49" s="0" t="n">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="L49" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="M49" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="50" spans="1:13">
+      <x:c r="A50" s="0" t="n">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="B50" s="0" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="C50" s="0" t="s">
+        <x:v>101</x:v>
+      </x:c>
+      <x:c r="D50" s="0" t="s">
+        <x:v>102</x:v>
+      </x:c>
+      <x:c r="E50" s="0" t="n">
+        <x:v>413</x:v>
+      </x:c>
+      <x:c r="F50" s="0" t="n">
+        <x:v>358</x:v>
+      </x:c>
+      <x:c r="G50" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="I50" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="J50" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="K50" s="0" t="n">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="L50" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="M50" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="51" spans="1:13">
+      <x:c r="A51" s="0" t="n">
+        <x:v>50</x:v>
+      </x:c>
+      <x:c r="B51" s="0" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="C51" s="0" t="s">
+        <x:v>102</x:v>
+      </x:c>
+      <x:c r="D51" s="0" t="s">
+        <x:v>103</x:v>
+      </x:c>
+      <x:c r="E51" s="0" t="n">
+        <x:v>541</x:v>
+      </x:c>
+      <x:c r="F51" s="0" t="n">
+        <x:v>384</x:v>
+      </x:c>
+      <x:c r="G51" s="0" t="n">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="H51" s="0" t="n">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="I51" s="0" t="n">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="J51" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="K51" s="0" t="n">
+        <x:v>39</x:v>
+      </x:c>
+      <x:c r="L51" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="M51" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="52" spans="1:13">
+      <x:c r="A52" s="0" t="n">
+        <x:v>51</x:v>
+      </x:c>
+      <x:c r="B52" s="0" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="C52" s="0" t="s">
+        <x:v>104</x:v>
+      </x:c>
+      <x:c r="D52" s="0" t="s">
+        <x:v>105</x:v>
+      </x:c>
+      <x:c r="E52" s="0" t="n">
+        <x:v>589</x:v>
+      </x:c>
+      <x:c r="F52" s="0" t="n">
+        <x:v>144</x:v>
+      </x:c>
+      <x:c r="G52" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="I52" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="J52" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="K52" s="0" t="n">
+        <x:v>39</x:v>
+      </x:c>
+      <x:c r="L52" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="M52" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="53" spans="1:13">
+      <x:c r="A53" s="0" t="n">
+        <x:v>52</x:v>
+      </x:c>
+      <x:c r="B53" s="0" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="C53" s="0" t="s">
+        <x:v>105</x:v>
+      </x:c>
+      <x:c r="D53" s="0" t="s">
+        <x:v>106</x:v>
+      </x:c>
+      <x:c r="E53" s="0" t="n">
+        <x:v>566</x:v>
+      </x:c>
+      <x:c r="F53" s="0" t="n">
+        <x:v>313</x:v>
+      </x:c>
+      <x:c r="G53" s="0" t="n">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="H53" s="0" t="n">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="I53" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="J53" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="K53" s="0" t="n">
+        <x:v>40</x:v>
+      </x:c>
+      <x:c r="L53" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="M53" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="54" spans="1:13">
+      <x:c r="A54" s="0" t="n">
+        <x:v>53</x:v>
+      </x:c>
+      <x:c r="B54" s="0" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="C54" s="0" t="s">
+        <x:v>107</x:v>
+      </x:c>
+      <x:c r="D54" s="0" t="s">
+        <x:v>108</x:v>
+      </x:c>
+      <x:c r="E54" s="0" t="n">
+        <x:v>615</x:v>
+      </x:c>
+      <x:c r="F54" s="0" t="n">
+        <x:v>328</x:v>
+      </x:c>
+      <x:c r="G54" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="I54" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="J54" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="K54" s="0" t="n">
+        <x:v>40</x:v>
+      </x:c>
+      <x:c r="L54" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="M54" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="55" spans="1:13">
+      <x:c r="A55" s="0" t="n">
+        <x:v>54</x:v>
+      </x:c>
+      <x:c r="B55" s="0" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="C55" s="0" t="s">
+        <x:v>108</x:v>
+      </x:c>
+      <x:c r="D55" s="0" t="s">
+        <x:v>109</x:v>
+      </x:c>
+      <x:c r="E55" s="0" t="n">
+        <x:v>593</x:v>
+      </x:c>
+      <x:c r="F55" s="0" t="n">
+        <x:v>371</x:v>
+      </x:c>
+      <x:c r="G55" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="I55" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="J55" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="K55" s="0" t="n">
+        <x:v>41</x:v>
+      </x:c>
+      <x:c r="L55" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="M55" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="56" spans="1:13">
+      <x:c r="A56" s="0" t="n">
+        <x:v>55</x:v>
+      </x:c>
+      <x:c r="B56" s="0" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="C56" s="0" t="s">
+        <x:v>110</x:v>
+      </x:c>
+      <x:c r="D56" s="0" t="s">
+        <x:v>111</x:v>
+      </x:c>
+      <x:c r="E56" s="0" t="n">
+        <x:v>347</x:v>
+      </x:c>
+      <x:c r="F56" s="0" t="n">
+        <x:v>388</x:v>
+      </x:c>
+      <x:c r="G56" s="0" t="n">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="H56" s="0" t="n">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="I56" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="J56" s="0" t="n">
+        <x:v>0.33</x:v>
+      </x:c>
+      <x:c r="K56" s="0" t="n">
+        <x:v>41</x:v>
+      </x:c>
+      <x:c r="L56" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="M56" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="57" spans="1:13">
+      <x:c r="A57" s="0" t="n">
+        <x:v>56</x:v>
+      </x:c>
+      <x:c r="B57" s="0" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="C57" s="0" t="s">
+        <x:v>111</x:v>
+      </x:c>
+      <x:c r="D57" s="0" t="s">
+        <x:v>112</x:v>
+      </x:c>
+      <x:c r="E57" s="0" t="n">
+        <x:v>373</x:v>
+      </x:c>
+      <x:c r="F57" s="0" t="n">
+        <x:v>278</x:v>
+      </x:c>
+      <x:c r="G57" s="0" t="n">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="H57" s="0" t="n">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="I57" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="J57" s="0" t="n">
+        <x:v>0.33</x:v>
+      </x:c>
+      <x:c r="K57" s="0" t="n">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="L57" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="M57" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="58" spans="1:13">
+      <x:c r="A58" s="0" t="n">
+        <x:v>57</x:v>
+      </x:c>
+      <x:c r="B58" s="0" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="C58" s="0" t="s">
+        <x:v>113</x:v>
+      </x:c>
+      <x:c r="D58" s="0" t="s">
+        <x:v>114</x:v>
+      </x:c>
+      <x:c r="E58" s="0" t="n">
+        <x:v>510</x:v>
+      </x:c>
+      <x:c r="F58" s="0" t="n">
+        <x:v>393</x:v>
+      </x:c>
+      <x:c r="G58" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="I58" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="J58" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="K58" s="0" t="n">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="L58" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="M58" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="59" spans="1:13">
+      <x:c r="A59" s="0" t="n">
+        <x:v>58</x:v>
+      </x:c>
+      <x:c r="B59" s="0" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="C59" s="0" t="s">
+        <x:v>115</x:v>
+      </x:c>
+      <x:c r="D59" s="0" t="s">
+        <x:v>116</x:v>
+      </x:c>
+      <x:c r="E59" s="0" t="n">
+        <x:v>503</x:v>
+      </x:c>
+      <x:c r="F59" s="0" t="n">
+        <x:v>357</x:v>
+      </x:c>
+      <x:c r="G59" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="I59" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="J59" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="K59" s="0" t="n">
+        <x:v>43</x:v>
+      </x:c>
+      <x:c r="L59" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="M59" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="60" spans="1:13">
+      <x:c r="A60" s="0" t="n">
+        <x:v>59</x:v>
+      </x:c>
+      <x:c r="B60" s="0" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="C60" s="0" t="s">
+        <x:v>117</x:v>
+      </x:c>
+      <x:c r="D60" s="0" t="s">
+        <x:v>118</x:v>
+      </x:c>
+      <x:c r="E60" s="0" t="n">
+        <x:v>518</x:v>
+      </x:c>
+      <x:c r="F60" s="0" t="n">
+        <x:v>384</x:v>
+      </x:c>
+      <x:c r="G60" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="I60" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="J60" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="K60" s="0" t="n">
+        <x:v>44</x:v>
+      </x:c>
+      <x:c r="L60" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="M60" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="61" spans="1:13">
+      <x:c r="A61" s="0" t="n">
+        <x:v>60</x:v>
+      </x:c>
+      <x:c r="B61" s="0" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="C61" s="0" t="s">
+        <x:v>119</x:v>
+      </x:c>
+      <x:c r="D61" s="0" t="s">
+        <x:v>120</x:v>
+      </x:c>
+      <x:c r="E61" s="0" t="n">
+        <x:v>547</x:v>
+      </x:c>
+      <x:c r="F61" s="0" t="n">
+        <x:v>505</x:v>
+      </x:c>
+      <x:c r="G61" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="I61" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="J61" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="K61" s="0" t="n">
+        <x:v>45</x:v>
+      </x:c>
+      <x:c r="L61" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="M61" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="62" spans="1:13">
+      <x:c r="A62" s="0" t="n">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="B62" s="0" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="C62" s="0" t="s">
+        <x:v>121</x:v>
+      </x:c>
+      <x:c r="D62" s="0" t="s">
+        <x:v>122</x:v>
+      </x:c>
+      <x:c r="E62" s="0" t="n">
+        <x:v>498</x:v>
+      </x:c>
+      <x:c r="F62" s="0" t="n">
+        <x:v>413</x:v>
+      </x:c>
+      <x:c r="G62" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="I62" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="J62" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="K62" s="0" t="n">
+        <x:v>46</x:v>
+      </x:c>
+      <x:c r="L62" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="M62" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="63" spans="1:13">
+      <x:c r="A63" s="0" t="n">
+        <x:v>62</x:v>
+      </x:c>
+      <x:c r="B63" s="0" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="C63" s="0" t="s">
+        <x:v>123</x:v>
+      </x:c>
+      <x:c r="D63" s="0" t="s">
+        <x:v>124</x:v>
+      </x:c>
+      <x:c r="E63" s="0" t="n">
+        <x:v>474</x:v>
+      </x:c>
+      <x:c r="F63" s="0" t="n">
+        <x:v>419</x:v>
+      </x:c>
+      <x:c r="G63" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="I63" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="J63" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="K63" s="0" t="n">
+        <x:v>47</x:v>
+      </x:c>
+      <x:c r="L63" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="M63" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="64" spans="1:13">
+      <x:c r="A64" s="0" t="n">
+        <x:v>63</x:v>
+      </x:c>
+      <x:c r="B64" s="0" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="C64" s="0" t="s">
+        <x:v>125</x:v>
+      </x:c>
+      <x:c r="D64" s="0" t="s">
+        <x:v>126</x:v>
+      </x:c>
+      <x:c r="G64" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="I64" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="J64" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="K64" s="0" t="n">
+        <x:v>48</x:v>
+      </x:c>
+      <x:c r="L64" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="M64" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="65" spans="1:13">
+      <x:c r="A65" s="0" t="n">
+        <x:v>64</x:v>
+      </x:c>
+      <x:c r="B65" s="0" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="C65" s="0" t="s">
+        <x:v>127</x:v>
+      </x:c>
+      <x:c r="D65" s="0" t="s">
+        <x:v>128</x:v>
+      </x:c>
+      <x:c r="E65" s="0" t="n">
+        <x:v>483</x:v>
+      </x:c>
+      <x:c r="F65" s="0" t="n">
+        <x:v>469</x:v>
+      </x:c>
+      <x:c r="G65" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="I65" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="J65" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="K65" s="0" t="n">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="L65" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="M65" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="66" spans="1:13">
+      <x:c r="A66" s="0" t="n">
+        <x:v>65</x:v>
+      </x:c>
+      <x:c r="B66" s="0" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="C66" s="0" t="s">
+        <x:v>129</x:v>
+      </x:c>
+      <x:c r="D66" s="0" t="s">
+        <x:v>130</x:v>
+      </x:c>
+      <x:c r="E66" s="0" t="n">
+        <x:v>629</x:v>
+      </x:c>
+      <x:c r="F66" s="0" t="n">
+        <x:v>206</x:v>
+      </x:c>
+      <x:c r="G66" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="I66" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="J66" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="K66" s="0" t="n">
+        <x:v>50</x:v>
+      </x:c>
+      <x:c r="L66" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="M66" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="67" spans="1:13">
+      <x:c r="A67" s="0" t="n">
+        <x:v>66</x:v>
+      </x:c>
+      <x:c r="B67" s="0" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="C67" s="0" t="s">
+        <x:v>130</x:v>
+      </x:c>
+      <x:c r="D67" s="0" t="s">
+        <x:v>131</x:v>
+      </x:c>
+      <x:c r="E67" s="0" t="n">
+        <x:v>465</x:v>
+      </x:c>
+      <x:c r="F67" s="0" t="n">
+        <x:v>93</x:v>
+      </x:c>
+      <x:c r="G67" s="0" t="n">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="H67" s="0" t="n">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="I67" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="J67" s="0" t="n">
+        <x:v>1.32</x:v>
+      </x:c>
+      <x:c r="K67" s="0" t="n">
+        <x:v>51</x:v>
+      </x:c>
+      <x:c r="L67" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="M67" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="68" spans="1:13">
+      <x:c r="A68" s="0" t="n">
+        <x:v>67</x:v>
+      </x:c>
+      <x:c r="B68" s="0" t="s">
+        <x:v>132</x:v>
+      </x:c>
+      <x:c r="C68" s="0" t="s">
+        <x:v>131</x:v>
+      </x:c>
+      <x:c r="D68" s="0" t="s">
+        <x:v>133</x:v>
+      </x:c>
+      <x:c r="E68" s="0" t="n">
+        <x:v>1059</x:v>
+      </x:c>
+      <x:c r="F68" s="0" t="n">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="G68" s="0" t="n">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="H68" s="0" t="n">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="I68" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="J68" s="0" t="n">
+        <x:v>0.33</x:v>
+      </x:c>
+      <x:c r="K68" s="0" t="n">
+        <x:v>51</x:v>
+      </x:c>
+      <x:c r="L68" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="M68" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="69" spans="1:13">
+      <x:c r="A69" s="0" t="n">
+        <x:v>68</x:v>
+      </x:c>
+      <x:c r="B69" s="0" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="C69" s="0" t="s">
+        <x:v>133</x:v>
+      </x:c>
+      <x:c r="D69" s="0" t="s">
+        <x:v>134</x:v>
+      </x:c>
+      <x:c r="E69" s="0" t="n">
+        <x:v>469</x:v>
+      </x:c>
+      <x:c r="F69" s="0" t="n">
+        <x:v>89</x:v>
+      </x:c>
+      <x:c r="G69" s="0" t="n">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="H69" s="0" t="n">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="I69" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="J69" s="0" t="n">
+        <x:v>0.33</x:v>
+      </x:c>
+      <x:c r="K69" s="0" t="n">
+        <x:v>51</x:v>
+      </x:c>
+      <x:c r="L69" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="M69" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="70" spans="1:13">
+      <x:c r="A70" s="0" t="n">
+        <x:v>69</x:v>
+      </x:c>
+      <x:c r="B70" s="0" t="s">
+        <x:v>132</x:v>
+      </x:c>
+      <x:c r="C70" s="0" t="s">
+        <x:v>134</x:v>
+      </x:c>
+      <x:c r="D70" s="0" t="s">
+        <x:v>135</x:v>
+      </x:c>
+      <x:c r="E70" s="0" t="n">
+        <x:v>1061</x:v>
+      </x:c>
+      <x:c r="F70" s="0" t="n">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="G70" s="0" t="n">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="H70" s="0" t="n">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="I70" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="J70" s="0" t="n">
+        <x:v>0.33</x:v>
+      </x:c>
+      <x:c r="K70" s="0" t="n">
+        <x:v>51</x:v>
+      </x:c>
+      <x:c r="L70" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="M70" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="71" spans="1:13">
+      <x:c r="A71" s="0" t="n">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="B71" s="0" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="C71" s="0" t="s">
+        <x:v>135</x:v>
+      </x:c>
+      <x:c r="D71" s="0" t="s">
+        <x:v>136</x:v>
+      </x:c>
+      <x:c r="E71" s="0" t="n">
+        <x:v>379</x:v>
+      </x:c>
+      <x:c r="F71" s="0" t="n">
+        <x:v>389</x:v>
+      </x:c>
+      <x:c r="G71" s="0" t="n">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="H71" s="0" t="n">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="I71" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="J71" s="0" t="n">
+        <x:v>0.33</x:v>
+      </x:c>
+      <x:c r="K71" s="0" t="n">
+        <x:v>51</x:v>
+      </x:c>
+      <x:c r="L71" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="M71" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="72" spans="1:13">
+      <x:c r="A72" s="0" t="n">
+        <x:v>71</x:v>
+      </x:c>
+      <x:c r="B72" s="0" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="C72" s="0" t="s">
+        <x:v>137</x:v>
+      </x:c>
+      <x:c r="D72" s="0" t="s">
+        <x:v>138</x:v>
+      </x:c>
+      <x:c r="E72" s="0" t="n">
+        <x:v>397</x:v>
+      </x:c>
+      <x:c r="F72" s="0" t="n">
+        <x:v>546</x:v>
+      </x:c>
+      <x:c r="G72" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="I72" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="J72" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="K72" s="0" t="n">
+        <x:v>51</x:v>
+      </x:c>
+      <x:c r="L72" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="M72" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="73" spans="1:13">
+      <x:c r="A73" s="0" t="n">
+        <x:v>72</x:v>
+      </x:c>
+      <x:c r="B73" s="0" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="C73" s="0" t="s">
+        <x:v>139</x:v>
+      </x:c>
+      <x:c r="D73" s="0" t="s">
+        <x:v>140</x:v>
+      </x:c>
+      <x:c r="E73" s="0" t="n">
+        <x:v>408</x:v>
+      </x:c>
+      <x:c r="F73" s="0" t="n">
+        <x:v>110</x:v>
+      </x:c>
+      <x:c r="G73" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="I73" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="J73" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="K73" s="0" t="n">
+        <x:v>52</x:v>
+      </x:c>
+      <x:c r="L73" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="M73" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="74" spans="1:13">
+      <x:c r="A74" s="0" t="n">
+        <x:v>73</x:v>
+      </x:c>
+      <x:c r="B74" s="0" t="s">
+        <x:v>132</x:v>
+      </x:c>
+      <x:c r="C74" s="0" t="s">
+        <x:v>141</x:v>
+      </x:c>
+      <x:c r="D74" s="0" t="s">
+        <x:v>142</x:v>
+      </x:c>
+      <x:c r="E74" s="0" t="n">
+        <x:v>351</x:v>
+      </x:c>
+      <x:c r="F74" s="0" t="n">
+        <x:v>173</x:v>
+      </x:c>
+      <x:c r="G74" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="I74" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="J74" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="K74" s="0" t="n">
+        <x:v>53</x:v>
+      </x:c>
+      <x:c r="L74" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="M74" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
   </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>

</xml_diff>